<commit_message>
Started the evaluation section of the singly linked list
</commit_message>
<xml_diff>
--- a/Data Structures/linked_list/Singly Linked List/Singly Linked_List.xlsx
+++ b/Data Structures/linked_list/Singly Linked List/Singly Linked_List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="83">
   <si>
     <t>Singly Linked List 128</t>
   </si>
@@ -245,6 +245,30 @@
   <si>
     <t>Cube (16 Core) Lockless</t>
   </si>
+  <si>
+    <t>Compare-and-swap</t>
+  </si>
+  <si>
+    <t>Test-and-set</t>
+  </si>
+  <si>
+    <t>Test-and-test-and-set</t>
+  </si>
+  <si>
+    <t>Cycles</t>
+  </si>
+  <si>
+    <t>Cache References</t>
+  </si>
+  <si>
+    <t>Cache Misses</t>
+  </si>
+  <si>
+    <t>Branches</t>
+  </si>
+  <si>
+    <t>Branch Misses</t>
+  </si>
 </sst>
 </file>
 
@@ -290,7 +314,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -302,10 +326,11 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -583,28 +608,28 @@
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1839686</c:v>
+                  <c:v>1851165</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6400983</c:v>
+                  <c:v>4336163</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5501337</c:v>
+                  <c:v>4299992</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6417378</c:v>
+                  <c:v>6857697</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1212031</c:v>
+                  <c:v>6875533</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1234938</c:v>
+                  <c:v>6922423</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3903148</c:v>
+                  <c:v>6993498</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2912524</c:v>
+                  <c:v>3116453</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -703,11 +728,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="97383936"/>
-        <c:axId val="97400320"/>
+        <c:axId val="105744256"/>
+        <c:axId val="105758720"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="97383936"/>
+        <c:axId val="105744256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -736,7 +761,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97400320"/>
+        <c:crossAx val="105758720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -744,7 +769,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="97400320"/>
+        <c:axId val="105758720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -774,7 +799,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97383936"/>
+        <c:crossAx val="105744256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1178,11 +1203,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="98920320"/>
-        <c:axId val="98941184"/>
+        <c:axId val="105597568"/>
+        <c:axId val="105603840"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="98920320"/>
+        <c:axId val="105597568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1211,7 +1236,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98941184"/>
+        <c:crossAx val="105603840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1219,7 +1244,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="98941184"/>
+        <c:axId val="105603840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1249,7 +1274,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98920320"/>
+        <c:crossAx val="105597568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1489,11 +1514,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="59022336"/>
-        <c:axId val="59176064"/>
+        <c:axId val="105637760"/>
+        <c:axId val="105639936"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="59022336"/>
+        <c:axId val="105637760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1522,7 +1547,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59176064"/>
+        <c:crossAx val="105639936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1530,7 +1555,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="59176064"/>
+        <c:axId val="105639936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1560,7 +1585,400 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59022336"/>
+        <c:crossAx val="105637760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-IE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-IE"/>
+              <a:t>Singly</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-IE" baseline="0"/>
+              <a:t> Linked List; Stoker; All Locks; 128 Key Range</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-IE"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Stoker (32 Core) CAS lock</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$R$22:$Y$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$R$23:$Y$23</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1771193</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4481236</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4253701</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3122722</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4925968</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2767640</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4615406</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4908164</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Stoker (32 Core) TAS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$R$22:$Y$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$R$24:$Y$24</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1003746</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1008307</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1013533</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1013987</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1021782</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1037191</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1063107</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1097845</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Stoker (32 Core) TTAS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$R$22:$Y$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$R$25:$Y$25</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1824016</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1346565</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1353986</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1354710</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1149411</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>926257</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>926629</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>949073</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="42398464"/>
+        <c:axId val="42400384"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="42398464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Threads</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="42400384"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="42400384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Iterations per second</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="42398464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1648,16 +2066,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>2295525</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>28576</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>123826</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>1362075</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>723901</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>104776</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1673,6 +2091,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>1009650</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>1019175</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1968,10 +2418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:X470"/>
+  <dimension ref="A4:AB470"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="Q238" activeCellId="1" sqref="L238:L239 Q238:Q239"/>
+    <sheetView tabSelected="1" topLeftCell="L13" workbookViewId="0">
+      <selection activeCell="R40" sqref="R40:W43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1988,10 +2438,11 @@
     <col min="15" max="15" width="14.7109375" customWidth="1"/>
     <col min="16" max="16" width="15.28515625" customWidth="1"/>
     <col min="17" max="17" width="24" customWidth="1"/>
-    <col min="18" max="18" width="14.7109375" customWidth="1"/>
+    <col min="18" max="18" width="17.7109375" customWidth="1"/>
     <col min="19" max="19" width="14.85546875" customWidth="1"/>
     <col min="22" max="22" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -2113,15 +2564,15 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -2188,28 +2639,28 @@
         <v>10</v>
       </c>
       <c r="B13" s="6">
-        <v>1839686</v>
+        <v>1851165</v>
       </c>
       <c r="C13" s="6">
-        <v>6400983</v>
+        <v>4336163</v>
       </c>
       <c r="D13" s="6">
-        <v>5501337</v>
+        <v>4299992</v>
       </c>
       <c r="E13" s="6">
-        <v>6417378</v>
+        <v>6857697</v>
       </c>
       <c r="F13" s="6">
-        <v>1212031</v>
+        <v>6875533</v>
       </c>
       <c r="G13" s="6">
-        <v>1234938</v>
+        <v>6922423</v>
       </c>
       <c r="H13" s="6">
-        <v>3903148</v>
+        <v>6993498</v>
       </c>
       <c r="I13" s="6">
-        <v>2912524</v>
+        <v>3116453</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -2299,7 +2750,7 @@
         <v>27924</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -2328,7 +2779,7 @@
         <v>300643</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -2357,7 +2808,7 @@
         <v>937594</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -2370,7 +2821,7 @@
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -2399,7 +2850,7 @@
         <v>353075</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -2428,7 +2879,7 @@
         <v>28346</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -2440,8 +2891,32 @@
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="R22">
+        <v>1</v>
+      </c>
+      <c r="S22">
+        <v>2</v>
+      </c>
+      <c r="T22">
+        <v>4</v>
+      </c>
+      <c r="U22">
+        <v>8</v>
+      </c>
+      <c r="V22">
+        <v>16</v>
+      </c>
+      <c r="W22">
+        <v>32</v>
+      </c>
+      <c r="X22">
+        <v>64</v>
+      </c>
+      <c r="Y22">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -2469,8 +2944,35 @@
       <c r="I23" s="6">
         <v>1367</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q23" t="s">
+        <v>10</v>
+      </c>
+      <c r="R23" s="6">
+        <v>1771193</v>
+      </c>
+      <c r="S23" s="6">
+        <v>4481236</v>
+      </c>
+      <c r="T23" s="6">
+        <v>4253701</v>
+      </c>
+      <c r="U23" s="6">
+        <v>3122722</v>
+      </c>
+      <c r="V23" s="6">
+        <v>4925968</v>
+      </c>
+      <c r="W23" s="6">
+        <v>2767640</v>
+      </c>
+      <c r="X23" s="6">
+        <v>4615406</v>
+      </c>
+      <c r="Y23" s="6">
+        <v>4908164</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -2498,8 +3000,35 @@
       <c r="I24" s="6">
         <v>382758</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q24" t="s">
+        <v>12</v>
+      </c>
+      <c r="R24" s="6">
+        <v>1003746</v>
+      </c>
+      <c r="S24" s="6">
+        <v>1008307</v>
+      </c>
+      <c r="T24" s="6">
+        <v>1013533</v>
+      </c>
+      <c r="U24" s="6">
+        <v>1013987</v>
+      </c>
+      <c r="V24" s="6">
+        <v>1021782</v>
+      </c>
+      <c r="W24" s="6">
+        <v>1037191</v>
+      </c>
+      <c r="X24" s="6">
+        <v>1063107</v>
+      </c>
+      <c r="Y24" s="6">
+        <v>1097845</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -2527,8 +3056,35 @@
       <c r="I25" s="6">
         <v>2943382</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q25" t="s">
+        <v>15</v>
+      </c>
+      <c r="R25" s="6">
+        <v>1824016</v>
+      </c>
+      <c r="S25" s="6">
+        <v>1346565</v>
+      </c>
+      <c r="T25" s="6">
+        <v>1353986</v>
+      </c>
+      <c r="U25" s="6">
+        <v>1354710</v>
+      </c>
+      <c r="V25" s="6">
+        <v>1149411</v>
+      </c>
+      <c r="W25" s="6">
+        <v>926257</v>
+      </c>
+      <c r="X25" s="6">
+        <v>926629</v>
+      </c>
+      <c r="Y25" s="6">
+        <v>949073</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -2557,7 +3113,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -2586,7 +3142,7 @@
         <v>2803987</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -2614,8 +3170,35 @@
       <c r="I28" s="6">
         <v>2348175</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q28" t="s">
+        <v>47</v>
+      </c>
+      <c r="R28" s="11">
+        <v>82558299728</v>
+      </c>
+      <c r="S28" t="s">
+        <v>35</v>
+      </c>
+      <c r="U28" t="s">
+        <v>51</v>
+      </c>
+      <c r="V28" s="11">
+        <v>73754753414</v>
+      </c>
+      <c r="W28" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z28" s="11">
+        <v>79283046259</v>
+      </c>
+      <c r="AA28" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -2643,8 +3226,26 @@
       <c r="I29" s="6">
         <v>2834344</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="R29" s="11">
+        <v>79993053916</v>
+      </c>
+      <c r="S29" t="s">
+        <v>36</v>
+      </c>
+      <c r="V29" s="11">
+        <v>73458421770</v>
+      </c>
+      <c r="W29" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z29" s="11">
+        <v>69425333770</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -2672,8 +3273,26 @@
       <c r="I30" s="6">
         <v>2791858</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="R30" s="11">
+        <v>36961822</v>
+      </c>
+      <c r="S30" t="s">
+        <v>37</v>
+      </c>
+      <c r="V30" s="11">
+        <v>37966386</v>
+      </c>
+      <c r="W30" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z30" s="11">
+        <v>25294826</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -2685,8 +3304,35 @@
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="R31" s="11">
+        <v>29457791</v>
+      </c>
+      <c r="S31" t="s">
+        <v>38</v>
+      </c>
+      <c r="T31">
+        <v>50.667236046021394</v>
+      </c>
+      <c r="V31" s="11">
+        <v>30268008</v>
+      </c>
+      <c r="W31" t="s">
+        <v>38</v>
+      </c>
+      <c r="X31">
+        <v>77.918622500978216</v>
+      </c>
+      <c r="Z31" s="11">
+        <v>18165651</v>
+      </c>
+      <c r="AA31" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB31">
+        <v>73.166653686548472</v>
+      </c>
+    </row>
+    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -2714,8 +3360,26 @@
       <c r="I32" s="6">
         <v>1895925</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="R32" s="11">
+        <v>14583767144</v>
+      </c>
+      <c r="S32" t="s">
+        <v>39</v>
+      </c>
+      <c r="V32" s="11">
+        <v>12986323663</v>
+      </c>
+      <c r="W32" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z32" s="11">
+        <v>13720399328</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -2743,8 +3407,35 @@
       <c r="I33" s="6">
         <v>2517295</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="R33" s="11">
+        <v>85001684</v>
+      </c>
+      <c r="S33" t="s">
+        <v>40</v>
+      </c>
+      <c r="T33">
+        <v>5.5695737849332259E-2</v>
+      </c>
+      <c r="V33" s="11">
+        <v>87687563</v>
+      </c>
+      <c r="W33" t="s">
+        <v>40</v>
+      </c>
+      <c r="X33">
+        <v>0.54227711554992397</v>
+      </c>
+      <c r="Z33" s="11">
+        <v>50788864</v>
+      </c>
+      <c r="AA33" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB33">
+        <v>0.26460802304224473</v>
+      </c>
+    </row>
+    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -2756,8 +3447,26 @@
       <c r="G34" s="6"/>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="R34" s="11">
+        <v>7447579029</v>
+      </c>
+      <c r="S34" t="s">
+        <v>41</v>
+      </c>
+      <c r="V34" s="11">
+        <v>7449660287</v>
+      </c>
+      <c r="W34" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z34" s="11">
+        <v>7443477175</v>
+      </c>
+      <c r="AA34" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -2785,8 +3494,26 @@
       <c r="I35" s="6">
         <v>2963781</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="R35" s="11">
+        <v>56541.019141999997</v>
+      </c>
+      <c r="S35" t="s">
+        <v>42</v>
+      </c>
+      <c r="V35" s="11">
+        <v>56551.893838999997</v>
+      </c>
+      <c r="W35" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z35" s="11">
+        <v>56507.986220999999</v>
+      </c>
+      <c r="AA35" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>54</v>
       </c>
@@ -2814,8 +3541,26 @@
       <c r="I36" s="6">
         <v>553487</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="R36" s="11">
+        <v>56541.287886999999</v>
+      </c>
+      <c r="S36" t="s">
+        <v>43</v>
+      </c>
+      <c r="V36" s="11">
+        <v>56552.991120999999</v>
+      </c>
+      <c r="W36" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z36" s="11">
+        <v>56508.155189999998</v>
+      </c>
+      <c r="AA36" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>55</v>
       </c>
@@ -2843,8 +3588,35 @@
       <c r="I37" s="6">
         <v>1319463</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="R37" s="11">
+        <v>53250730840</v>
+      </c>
+      <c r="S37" t="s">
+        <v>44</v>
+      </c>
+      <c r="T37">
+        <v>88.749483220808813</v>
+      </c>
+      <c r="V37" s="11">
+        <v>47451561515</v>
+      </c>
+      <c r="W37" t="s">
+        <v>44</v>
+      </c>
+      <c r="X37">
+        <v>64.184005504861759</v>
+      </c>
+      <c r="Z37" s="11">
+        <v>51107363705</v>
+      </c>
+      <c r="AA37" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB37">
+        <v>64.265241130843222</v>
+      </c>
+    </row>
+    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>56</v>
       </c>
@@ -2872,8 +3644,35 @@
       <c r="I38" s="7">
         <v>173</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="R38" s="11">
+        <v>16853118796</v>
+      </c>
+      <c r="S38" t="s">
+        <v>45</v>
+      </c>
+      <c r="T38">
+        <v>45.999796145462902</v>
+      </c>
+      <c r="V38" s="11">
+        <v>19804503959</v>
+      </c>
+      <c r="W38" t="s">
+        <v>45</v>
+      </c>
+      <c r="X38">
+        <v>25.996948385166341</v>
+      </c>
+      <c r="Z38" s="11">
+        <v>28746549934</v>
+      </c>
+      <c r="AA38" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB38">
+        <v>36.865107953874791</v>
+      </c>
+    </row>
+    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>57</v>
       </c>
@@ -2902,7 +3701,7 @@
         <v>1326474</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>58</v>
       </c>
@@ -2930,8 +3729,23 @@
       <c r="I40" s="6">
         <v>73838</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="S40" t="s">
+        <v>78</v>
+      </c>
+      <c r="T40" t="s">
+        <v>79</v>
+      </c>
+      <c r="U40" t="s">
+        <v>80</v>
+      </c>
+      <c r="V40" t="s">
+        <v>81</v>
+      </c>
+      <c r="W40" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="41" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>59</v>
       </c>
@@ -2959,8 +3773,26 @@
       <c r="I41" s="6">
         <v>173395</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="R41" t="s">
+        <v>75</v>
+      </c>
+      <c r="S41" s="11">
+        <v>79283046259</v>
+      </c>
+      <c r="T41" s="11">
+        <v>25294826</v>
+      </c>
+      <c r="U41" s="11">
+        <v>18165651</v>
+      </c>
+      <c r="V41" s="11">
+        <v>13720399328</v>
+      </c>
+      <c r="W41" s="11">
+        <v>50788864</v>
+      </c>
+    </row>
+    <row r="42" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>60</v>
       </c>
@@ -2988,8 +3820,26 @@
       <c r="I42" s="6">
         <v>1326632</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="R42" t="s">
+        <v>76</v>
+      </c>
+      <c r="S42" s="11">
+        <v>73754753414</v>
+      </c>
+      <c r="T42" s="11">
+        <v>37966386</v>
+      </c>
+      <c r="U42" s="11">
+        <v>30268008</v>
+      </c>
+      <c r="V42" s="11">
+        <v>12986323663</v>
+      </c>
+      <c r="W42" s="11">
+        <v>87687563</v>
+      </c>
+    </row>
+    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>61</v>
       </c>
@@ -3001,8 +3851,26 @@
       <c r="G43" s="6"/>
       <c r="H43" s="6"/>
       <c r="I43" s="6"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="R43" t="s">
+        <v>77</v>
+      </c>
+      <c r="S43" s="11">
+        <v>82558299728</v>
+      </c>
+      <c r="T43" s="11">
+        <v>36961822</v>
+      </c>
+      <c r="U43" s="11">
+        <v>29457791</v>
+      </c>
+      <c r="V43" s="11">
+        <v>14583767144</v>
+      </c>
+      <c r="W43" s="11">
+        <v>85001684</v>
+      </c>
+    </row>
+    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>62</v>
       </c>
@@ -3031,7 +3899,7 @@
         <v>229328</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>63</v>
       </c>
@@ -3060,7 +3928,7 @@
         <v>85934</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>64</v>
       </c>
@@ -3073,7 +3941,7 @@
       <c r="H46" s="6"/>
       <c r="I46" s="6"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>65</v>
       </c>
@@ -3103,15 +3971,15 @@
       </c>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A50" s="9"/>
-      <c r="B50" s="9"/>
-      <c r="C50" s="9"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="9"/>
-      <c r="G50" s="9"/>
-      <c r="H50" s="9"/>
-      <c r="I50" s="9"/>
+      <c r="A50" s="10"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="10"/>
+      <c r="G50" s="10"/>
+      <c r="H50" s="10"/>
+      <c r="I50" s="10"/>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
@@ -3452,7 +4320,7 @@
       <c r="I64" s="6"/>
       <c r="L64" s="5"/>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>22</v>
       </c>
@@ -3481,8 +4349,9 @@
         <v>13080</v>
       </c>
       <c r="L65" s="1"/>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="V65" s="3"/>
+    </row>
+    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>23</v>
       </c>
@@ -3496,7 +4365,7 @@
       <c r="I66" s="6"/>
       <c r="L66" s="1"/>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>24</v>
       </c>
@@ -3511,7 +4380,7 @@
       <c r="L67" s="1"/>
       <c r="O67" s="2"/>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>25</v>
       </c>
@@ -3526,7 +4395,7 @@
       <c r="L68" s="1"/>
       <c r="O68" s="2"/>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>26</v>
       </c>
@@ -3555,7 +4424,7 @@
         <v>9685</v>
       </c>
     </row>
-    <row r="70" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>27</v>
       </c>
@@ -3584,8 +4453,9 @@
         <v>11996</v>
       </c>
       <c r="L70" s="5"/>
-    </row>
-    <row r="71" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V70"/>
+    </row>
+    <row r="71" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>28</v>
       </c>
@@ -3614,7 +4484,7 @@
         <v>9605</v>
       </c>
     </row>
-    <row r="72" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>29</v>
       </c>
@@ -3628,7 +4498,7 @@
       <c r="I72" s="6"/>
       <c r="L72" s="5"/>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>30</v>
       </c>
@@ -3658,8 +4528,9 @@
       </c>
       <c r="L73" s="1"/>
       <c r="O73" s="2"/>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="V73" s="3"/>
+    </row>
+    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>31</v>
       </c>
@@ -3674,7 +4545,7 @@
       <c r="L74" s="1"/>
       <c r="O74" s="2"/>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>32</v>
       </c>
@@ -3689,7 +4560,7 @@
       <c r="L75" s="1"/>
       <c r="O75" s="2"/>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>33</v>
       </c>
@@ -3704,7 +4575,7 @@
       <c r="L76" s="1"/>
       <c r="O76" s="2"/>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>54</v>
       </c>
@@ -3733,7 +4604,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>55</v>
       </c>
@@ -3746,7 +4617,7 @@
       <c r="H78" s="6"/>
       <c r="I78" s="6"/>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>56</v>
       </c>
@@ -3759,7 +4630,7 @@
       <c r="H79" s="7"/>
       <c r="I79" s="7"/>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>57</v>
       </c>
@@ -4029,15 +4900,15 @@
       </c>
     </row>
     <row r="93" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A93" s="9"/>
-      <c r="B93" s="9"/>
-      <c r="C93" s="9"/>
-      <c r="D93" s="9"/>
-      <c r="E93" s="9"/>
-      <c r="F93" s="9"/>
-      <c r="G93" s="9"/>
-      <c r="H93" s="9"/>
-      <c r="I93" s="9"/>
+      <c r="A93" s="10"/>
+      <c r="B93" s="10"/>
+      <c r="C93" s="10"/>
+      <c r="D93" s="10"/>
+      <c r="E93" s="10"/>
+      <c r="F93" s="10"/>
+      <c r="G93" s="10"/>
+      <c r="H93" s="10"/>
+      <c r="I93" s="10"/>
       <c r="K93" t="s">
         <v>9</v>
       </c>
@@ -6828,7 +7699,7 @@
       <c r="K236" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="L236" s="10">
+      <c r="L236" s="9">
         <v>2320251390985</v>
       </c>
       <c r="M236" s="6" t="s">
@@ -6849,9 +7720,6 @@
       <c r="T236" s="6"/>
       <c r="U236" s="6" t="s">
         <v>47</v>
-      </c>
-      <c r="V236" s="6">
-        <v>2719592214572</v>
       </c>
       <c r="W236" s="6" t="s">
         <v>35</v>
@@ -6900,7 +7768,7 @@
       <c r="T237" s="6"/>
       <c r="U237" s="6"/>
       <c r="V237" s="6">
-        <v>587651715850</v>
+        <v>2719592214572</v>
       </c>
       <c r="W237" s="6" t="s">
         <v>36</v>
@@ -6930,7 +7798,7 @@
         <v>23.706980674482296</v>
       </c>
       <c r="K238" s="6"/>
-      <c r="L238" s="10">
+      <c r="L238" s="9">
         <v>920908737</v>
       </c>
       <c r="M238" s="6" t="s">
@@ -6939,7 +7807,7 @@
       <c r="N238" s="6"/>
       <c r="O238" s="6"/>
       <c r="P238" s="6"/>
-      <c r="Q238" s="10">
+      <c r="Q238" s="9">
         <v>481953979</v>
       </c>
       <c r="R238" s="6" t="s">
@@ -6949,7 +7817,7 @@
       <c r="T238" s="6"/>
       <c r="U238" s="6"/>
       <c r="V238" s="6">
-        <v>543145791</v>
+        <v>587651715850</v>
       </c>
       <c r="W238" s="6" t="s">
         <v>37</v>
@@ -6965,7 +7833,7 @@
       <c r="H239" s="8"/>
       <c r="I239" s="8"/>
       <c r="K239" s="6"/>
-      <c r="L239" s="10">
+      <c r="L239" s="9">
         <v>376461981</v>
       </c>
       <c r="M239" s="6" t="s">
@@ -6977,7 +7845,7 @@
       </c>
       <c r="O239" s="6"/>
       <c r="P239" s="6"/>
-      <c r="Q239" s="10">
+      <c r="Q239" s="9">
         <v>248623295</v>
       </c>
       <c r="R239" s="6" t="s">
@@ -6990,13 +7858,13 @@
       <c r="T239" s="6"/>
       <c r="U239" s="6"/>
       <c r="V239" s="6">
-        <v>275196960</v>
+        <v>543145791</v>
       </c>
       <c r="W239" s="6" t="s">
         <v>38</v>
       </c>
       <c r="X239" s="6">
-        <f>V239/V238*100</f>
+        <f>V240/V239*100</f>
         <v>50.667236046021394</v>
       </c>
     </row>
@@ -7040,7 +7908,7 @@
       <c r="T240" s="6"/>
       <c r="U240" s="6"/>
       <c r="V240" s="6">
-        <v>196795694307</v>
+        <v>275196960</v>
       </c>
       <c r="W240" s="6" t="s">
         <v>39</v>
@@ -7086,13 +7954,13 @@
       <c r="T241" s="6"/>
       <c r="U241" s="6"/>
       <c r="V241" s="6">
-        <v>109606814</v>
+        <v>196795694307</v>
       </c>
       <c r="W241" s="6" t="s">
         <v>40</v>
       </c>
       <c r="X241" s="6">
-        <f>V241/V240*100</f>
+        <f>V242/V241*100</f>
         <v>5.5695737849332259E-2</v>
       </c>
     </row>
@@ -7129,7 +7997,7 @@
       <c r="T242" s="6"/>
       <c r="U242" s="6"/>
       <c r="V242" s="6">
-        <v>172475484924</v>
+        <v>109606814</v>
       </c>
       <c r="W242" s="6" t="s">
         <v>41</v>
@@ -7177,7 +8045,7 @@
       <c r="T243" s="6"/>
       <c r="U243" s="6"/>
       <c r="V243" s="6">
-        <v>1303150.86182</v>
+        <v>172475484924</v>
       </c>
       <c r="W243" s="6" t="s">
         <v>42</v>
@@ -7217,7 +8085,7 @@
       <c r="T244" s="6"/>
       <c r="U244" s="6"/>
       <c r="V244" s="6">
-        <v>1303149.8870560001</v>
+        <v>1303150.86182</v>
       </c>
       <c r="W244" s="6" t="s">
         <v>43</v>
@@ -7271,13 +8139,13 @@
       <c r="T245" s="6"/>
       <c r="U245" s="6"/>
       <c r="V245" s="6">
-        <v>2413624036146</v>
+        <v>1303149.8870560001</v>
       </c>
       <c r="W245" s="6" t="s">
         <v>44</v>
       </c>
       <c r="X245" s="6">
-        <f>V245/V236*100</f>
+        <f>V246/V237*100</f>
         <v>88.749483220808813</v>
       </c>
     </row>
@@ -7295,7 +8163,7 @@
         <v>41</v>
       </c>
       <c r="K246" s="6"/>
-      <c r="L246" s="10">
+      <c r="L246" s="9">
         <v>1373819293598</v>
       </c>
       <c r="M246" s="6" t="s">
@@ -7320,13 +8188,13 @@
       <c r="T246" s="6"/>
       <c r="U246" s="6"/>
       <c r="V246" s="6">
-        <v>1251006874691</v>
+        <v>2413624036146</v>
       </c>
       <c r="W246" s="6" t="s">
         <v>45</v>
       </c>
       <c r="X246" s="6">
-        <f>V246/V236*100</f>
+        <f>V247/V237*100</f>
         <v>45.999796145462902</v>
       </c>
     </row>
@@ -7354,7 +8222,9 @@
       <c r="S247" s="6"/>
       <c r="T247" s="6"/>
       <c r="U247" s="6"/>
-      <c r="V247" s="6"/>
+      <c r="V247" s="6">
+        <v>1251006874691</v>
+      </c>
       <c r="W247" s="6"/>
       <c r="X247" s="6"/>
     </row>
@@ -7371,6 +8241,7 @@
       <c r="H248" t="s">
         <v>43</v>
       </c>
+      <c r="V248" s="6"/>
     </row>
     <row r="249" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B249" s="1">

</xml_diff>

<commit_message>
Finished Singly linked list
</commit_message>
<xml_diff>
--- a/Data Structures/linked_list/Singly Linked List/Singly Linked_List.xlsx
+++ b/Data Structures/linked_list/Singly Linked List/Singly Linked_List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="91">
   <si>
     <t>Singly Linked List 128</t>
   </si>
@@ -360,9 +360,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -370,6 +367,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -767,11 +767,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="98666752"/>
-        <c:axId val="98681216"/>
+        <c:axId val="106137856"/>
+        <c:axId val="106148224"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="98666752"/>
+        <c:axId val="106137856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -800,7 +800,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98681216"/>
+        <c:crossAx val="106148224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -808,7 +808,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="98681216"/>
+        <c:axId val="106148224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -838,7 +838,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98666752"/>
+        <c:crossAx val="106137856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1078,11 +1078,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="112355200"/>
-        <c:axId val="112357376"/>
+        <c:axId val="107568512"/>
+        <c:axId val="107587072"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="112355200"/>
+        <c:axId val="107568512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1111,7 +1111,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112357376"/>
+        <c:crossAx val="107587072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1119,7 +1119,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112357376"/>
+        <c:axId val="107587072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1149,7 +1149,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112355200"/>
+        <c:crossAx val="107568512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -1474,11 +1474,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="112400256"/>
-        <c:axId val="112402432"/>
+        <c:axId val="107626496"/>
+        <c:axId val="107628416"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="112400256"/>
+        <c:axId val="107626496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1507,7 +1507,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112402432"/>
+        <c:crossAx val="107628416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1515,7 +1515,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112402432"/>
+        <c:axId val="107628416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1545,7 +1545,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112400256"/>
+        <c:crossAx val="107626496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -1870,11 +1870,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="112449408"/>
-        <c:axId val="112455680"/>
+        <c:axId val="107676032"/>
+        <c:axId val="107677952"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="112449408"/>
+        <c:axId val="107676032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1903,7 +1903,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112455680"/>
+        <c:crossAx val="107677952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1911,7 +1911,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112455680"/>
+        <c:axId val="107677952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1941,7 +1941,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112449408"/>
+        <c:crossAx val="107676032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -2266,11 +2266,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="112494464"/>
-        <c:axId val="112500736"/>
+        <c:axId val="107717376"/>
+        <c:axId val="107719296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="112494464"/>
+        <c:axId val="107717376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2299,7 +2299,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112500736"/>
+        <c:crossAx val="107719296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2307,7 +2307,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112500736"/>
+        <c:axId val="107719296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2337,12 +2337,948 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112494464"/>
+        <c:crossAx val="107717376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
           <c:builtInUnit val="millions"/>
         </c:dispUnits>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-IE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-IE"/>
+              <a:t>Singly</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-IE" baseline="0"/>
+              <a:t> Linked List; Stoker; Pthread Mutex Lock vs Lockless; 131072 Key Range</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-IE"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$V$109</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Stoker (32 Core) 131072 Lockless</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$W$107:$AD$107</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$W$109:$AD$109</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>3503</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3364</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5425</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8337</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13407</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23888</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40767</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>38376</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$V$110</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Stoker (32 Core) 131072 Locked</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$W$107:$AD$107</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$W$110:$AD$110</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>3346</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1404</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1046</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1351</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1113</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>848</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1082</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>976</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="40408960"/>
+        <c:axId val="40989824"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="40408960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Threads</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="40989824"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="40989824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Iterations per second</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="40408960"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-IE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-IE"/>
+              <a:t>Singly</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-IE" baseline="0"/>
+              <a:t> Linked List; Stoker; Pthread Mutex Lock vs Lockless; 128 Key Range</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-IE"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AE$107</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Stoker (32 Core) Lockless</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$AF$106:$AM$106</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AF$107:$AM$107</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>3457942</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3416827</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7830031</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3385509</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>868520</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>817838</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>830026</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>933362</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AE$108</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Stoker (32 Core) Locked</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$AF$106:$AM$106</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AF$108:$AM$108</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1838813</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1690111</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1007093</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>730487</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>267862</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>243491</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>226570</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>233753</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="50060288"/>
+        <c:axId val="71592576"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="50060288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Threads</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="71592576"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="71592576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Millions of Iterations per second</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50060288"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:dispUnits>
+          <c:builtInUnit val="millions"/>
+        </c:dispUnits>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-IE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-IE"/>
+              <a:t>Singly</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-IE" baseline="0"/>
+              <a:t> Linked List; Stoker; Pthread Mutex Lock vs Lockless; 128 Key Range</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-IE"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AP$107</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Stoker (32 Core) Locked</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$AQ$106:$AX$106</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AQ$107:$AX$107</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>3081</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1253</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>775</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>968</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>902</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>760</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>706</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>598</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AP$108</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Stoker (32 Core) Lockless</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$AQ$106:$AX$106</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AQ$108:$AX$108</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>3221</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2827</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3832</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5407</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7180</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10164</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13132</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10299</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="41891712"/>
+        <c:axId val="41951616"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="41891712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Threads</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="41951616"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="41951616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Millions of Iterations per second</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="41891712"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2744,11 +3680,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="99183616"/>
-        <c:axId val="99193984"/>
+        <c:axId val="106322944"/>
+        <c:axId val="106329216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="99183616"/>
+        <c:axId val="106322944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2777,7 +3713,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99193984"/>
+        <c:crossAx val="106329216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2785,7 +3721,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="99193984"/>
+        <c:axId val="106329216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2815,7 +3751,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99183616"/>
+        <c:crossAx val="106322944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3055,11 +3991,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="99219712"/>
-        <c:axId val="99221888"/>
+        <c:axId val="106359040"/>
+        <c:axId val="106365312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="99219712"/>
+        <c:axId val="106359040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3088,7 +4024,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99221888"/>
+        <c:crossAx val="106365312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3096,7 +4032,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="99221888"/>
+        <c:axId val="106365312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3126,7 +4062,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99219712"/>
+        <c:crossAx val="106359040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3458,11 +4394,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="99260672"/>
-        <c:axId val="99262848"/>
+        <c:axId val="106404096"/>
+        <c:axId val="106406272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="99260672"/>
+        <c:axId val="106404096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3491,7 +4427,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99262848"/>
+        <c:crossAx val="106406272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3499,7 +4435,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="99262848"/>
+        <c:axId val="106406272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3529,7 +4465,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99260672"/>
+        <c:crossAx val="106404096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -3936,11 +4872,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="99697792"/>
-        <c:axId val="99699712"/>
+        <c:axId val="106636416"/>
+        <c:axId val="106638336"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="99697792"/>
+        <c:axId val="106636416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3969,7 +4905,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99699712"/>
+        <c:crossAx val="106638336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3977,7 +4913,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="99699712"/>
+        <c:axId val="106638336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4007,7 +4943,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99697792"/>
+        <c:crossAx val="106636416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -4332,11 +5268,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="99734656"/>
-        <c:axId val="99736576"/>
+        <c:axId val="106692608"/>
+        <c:axId val="106694528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="99734656"/>
+        <c:axId val="106692608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4365,7 +5301,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99736576"/>
+        <c:crossAx val="106694528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4373,7 +5309,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="99736576"/>
+        <c:axId val="106694528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4403,7 +5339,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99734656"/>
+        <c:crossAx val="106692608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -4728,11 +5664,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="99771520"/>
-        <c:axId val="99773440"/>
+        <c:axId val="106725760"/>
+        <c:axId val="106727680"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="99771520"/>
+        <c:axId val="106725760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4761,7 +5697,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99773440"/>
+        <c:crossAx val="106727680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4769,7 +5705,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="99773440"/>
+        <c:axId val="106727680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4799,7 +5735,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99771520"/>
+        <c:crossAx val="106725760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5039,11 +5975,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="112601344"/>
-        <c:axId val="112607616"/>
+        <c:axId val="107486592"/>
+        <c:axId val="107488768"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="112601344"/>
+        <c:axId val="107486592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5072,7 +6008,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112607616"/>
+        <c:crossAx val="107488768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5080,7 +6016,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112607616"/>
+        <c:axId val="107488768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5110,7 +6046,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112601344"/>
+        <c:crossAx val="107486592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -5517,11 +6453,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="112646784"/>
-        <c:axId val="112329472"/>
+        <c:axId val="107549056"/>
+        <c:axId val="107550976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="112646784"/>
+        <c:axId val="107549056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5550,7 +6486,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112329472"/>
+        <c:crossAx val="107550976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5558,7 +6494,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112329472"/>
+        <c:axId val="107550976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5588,7 +6524,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112646784"/>
+        <c:crossAx val="107549056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5677,15 +6613,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>28576</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>123826</xdr:rowOff>
+      <xdr:colOff>228601</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>161926</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>723901</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>104776</xdr:rowOff>
+      <xdr:colOff>923926</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>142876</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6026,6 +6962,102 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>1343025</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="15" name="Chart 14"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="16" name="Chart 15"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="17" name="Chart 16"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId16"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6318,8 +7350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:BW470"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BG1" workbookViewId="0">
-      <selection activeCell="BY28" sqref="BY28"/>
+    <sheetView tabSelected="1" topLeftCell="T85" workbookViewId="0">
+      <selection activeCell="AP88" sqref="AP88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6474,15 +7506,15 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
+      <c r="A9" s="18"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -8778,14 +9810,14 @@
         <f>AE38/AE28*100</f>
         <v>59.209932981218131</v>
       </c>
-      <c r="AO38" s="16"/>
-      <c r="AP38" s="16"/>
-      <c r="AQ38" s="16"/>
-      <c r="AR38" s="16"/>
-      <c r="AS38" s="16"/>
-      <c r="AT38" s="16"/>
-      <c r="AU38" s="16"/>
-      <c r="AV38" s="16"/>
+      <c r="AO38" s="15"/>
+      <c r="AP38" s="15"/>
+      <c r="AQ38" s="15"/>
+      <c r="AR38" s="15"/>
+      <c r="AS38" s="15"/>
+      <c r="AT38" s="15"/>
+      <c r="AU38" s="15"/>
+      <c r="AV38" s="15"/>
     </row>
     <row r="39" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -8815,26 +9847,26 @@
       <c r="I39" s="6">
         <v>1326474</v>
       </c>
-      <c r="AO39" s="16"/>
-      <c r="AP39" s="16" t="s">
+      <c r="AO39" s="15"/>
+      <c r="AP39" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="AQ39" s="16" t="s">
+      <c r="AQ39" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="AR39" s="16" t="s">
+      <c r="AR39" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="AS39" s="16" t="s">
+      <c r="AS39" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="AT39" s="16" t="s">
+      <c r="AT39" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="AU39" s="16" t="s">
+      <c r="AU39" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="AV39" s="16" t="s">
+      <c r="AV39" s="15" t="s">
         <v>87</v>
       </c>
     </row>
@@ -8881,28 +9913,28 @@
       <c r="W40" t="s">
         <v>82</v>
       </c>
-      <c r="AO40" s="16" t="s">
+      <c r="AO40" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="AP40" s="17">
+      <c r="AP40" s="16">
         <v>81130469279</v>
       </c>
-      <c r="AQ40" s="18">
+      <c r="AQ40" s="17">
         <v>38564769</v>
       </c>
-      <c r="AR40" s="18">
+      <c r="AR40" s="17">
         <v>30639919</v>
       </c>
-      <c r="AS40" s="17">
+      <c r="AS40" s="16">
         <v>14209964743</v>
       </c>
-      <c r="AT40" s="18">
+      <c r="AT40" s="17">
         <v>88335935</v>
       </c>
-      <c r="AU40" s="17">
+      <c r="AU40" s="16">
         <v>52226598350</v>
       </c>
-      <c r="AV40" s="17">
+      <c r="AV40" s="16">
         <v>12480857829</v>
       </c>
     </row>
@@ -8937,43 +9969,43 @@
       <c r="R41" t="s">
         <v>75</v>
       </c>
-      <c r="S41" s="12">
+      <c r="S41" s="11">
         <v>79283046259</v>
       </c>
-      <c r="T41" s="14">
+      <c r="T41" s="13">
         <v>25294826</v>
       </c>
-      <c r="U41" s="14">
+      <c r="U41" s="13">
         <v>18165651</v>
       </c>
-      <c r="V41" s="12">
+      <c r="V41" s="11">
         <v>13720399328</v>
       </c>
-      <c r="W41" s="14">
+      <c r="W41" s="13">
         <v>50788864</v>
       </c>
-      <c r="AO41" s="16" t="s">
+      <c r="AO41" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="AP41" s="17">
+      <c r="AP41" s="16">
         <v>2668937427093</v>
       </c>
-      <c r="AQ41" s="18">
+      <c r="AQ41" s="17">
         <v>553205489</v>
       </c>
-      <c r="AR41" s="18">
+      <c r="AR41" s="17">
         <v>279018701</v>
       </c>
-      <c r="AS41" s="17">
+      <c r="AS41" s="16">
         <v>146423924590</v>
       </c>
-      <c r="AT41" s="18">
+      <c r="AT41" s="17">
         <v>98945050</v>
       </c>
-      <c r="AU41" s="17">
+      <c r="AU41" s="16">
         <v>2380557129188</v>
       </c>
-      <c r="AV41" s="17">
+      <c r="AV41" s="16">
         <v>1268953272943</v>
       </c>
     </row>
@@ -9008,43 +10040,43 @@
       <c r="R42" t="s">
         <v>76</v>
       </c>
-      <c r="S42" s="12">
+      <c r="S42" s="11">
         <v>73754753414</v>
       </c>
-      <c r="T42" s="14">
+      <c r="T42" s="13">
         <v>37966386</v>
       </c>
-      <c r="U42" s="14">
+      <c r="U42" s="13">
         <v>30268008</v>
       </c>
-      <c r="V42" s="12">
+      <c r="V42" s="11">
         <v>12986323663</v>
       </c>
-      <c r="W42" s="14">
+      <c r="W42" s="13">
         <v>87687563</v>
       </c>
-      <c r="AO42" s="16" t="s">
+      <c r="AO42" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="AP42" s="17">
+      <c r="AP42" s="16">
         <v>2694259174154</v>
       </c>
-      <c r="AQ42" s="18">
+      <c r="AQ42" s="17">
         <v>471658813</v>
       </c>
-      <c r="AR42" s="18">
+      <c r="AR42" s="17">
         <v>243422945</v>
       </c>
-      <c r="AS42" s="17">
+      <c r="AS42" s="16">
         <v>40191840648</v>
       </c>
-      <c r="AT42" s="18">
+      <c r="AT42" s="17">
         <v>91780840</v>
       </c>
-      <c r="AU42" s="17">
+      <c r="AU42" s="16">
         <v>2597363092991</v>
       </c>
-      <c r="AV42" s="17">
+      <c r="AV42" s="16">
         <v>2314939522901</v>
       </c>
     </row>
@@ -9063,19 +10095,19 @@
       <c r="R43" t="s">
         <v>77</v>
       </c>
-      <c r="S43" s="12">
+      <c r="S43" s="11">
         <v>82558299728</v>
       </c>
-      <c r="T43" s="14">
+      <c r="T43" s="13">
         <v>36961822</v>
       </c>
-      <c r="U43" s="14">
+      <c r="U43" s="13">
         <v>29457791</v>
       </c>
-      <c r="V43" s="12">
+      <c r="V43" s="11">
         <v>14583767144</v>
       </c>
-      <c r="W43" s="14">
+      <c r="W43" s="13">
         <v>85001684</v>
       </c>
       <c r="AP43" s="9"/>
@@ -9115,19 +10147,19 @@
       <c r="R44" t="s">
         <v>83</v>
       </c>
-      <c r="S44" s="13">
+      <c r="S44" s="12">
         <v>2320251390985</v>
       </c>
-      <c r="T44" s="15">
+      <c r="T44" s="14">
         <v>920908737</v>
       </c>
-      <c r="U44" s="15">
+      <c r="U44" s="14">
         <v>376461981</v>
       </c>
-      <c r="V44" s="13">
+      <c r="V44" s="12">
         <v>85035305784</v>
       </c>
-      <c r="W44" s="15">
+      <c r="W44" s="14">
         <v>177461291</v>
       </c>
     </row>
@@ -9203,15 +10235,15 @@
       </c>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A50" s="11"/>
-      <c r="B50" s="11"/>
-      <c r="C50" s="11"/>
-      <c r="D50" s="11"/>
-      <c r="E50" s="11"/>
-      <c r="F50" s="11"/>
-      <c r="G50" s="11"/>
-      <c r="H50" s="11"/>
-      <c r="I50" s="11"/>
+      <c r="A50" s="18"/>
+      <c r="B50" s="18"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="18"/>
+      <c r="F50" s="18"/>
+      <c r="G50" s="18"/>
+      <c r="H50" s="18"/>
+      <c r="I50" s="18"/>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
@@ -10132,15 +11164,15 @@
       </c>
     </row>
     <row r="93" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A93" s="11"/>
-      <c r="B93" s="11"/>
-      <c r="C93" s="11"/>
-      <c r="D93" s="11"/>
-      <c r="E93" s="11"/>
-      <c r="F93" s="11"/>
-      <c r="G93" s="11"/>
-      <c r="H93" s="11"/>
-      <c r="I93" s="11"/>
+      <c r="A93" s="18"/>
+      <c r="B93" s="18"/>
+      <c r="C93" s="18"/>
+      <c r="D93" s="18"/>
+      <c r="E93" s="18"/>
+      <c r="F93" s="18"/>
+      <c r="G93" s="18"/>
+      <c r="H93" s="18"/>
+      <c r="I93" s="18"/>
       <c r="K93" t="s">
         <v>9</v>
       </c>
@@ -10285,7 +11317,7 @@
       <c r="L96" s="1"/>
       <c r="O96" s="2"/>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>10</v>
       </c>
@@ -10316,7 +11348,7 @@
       <c r="L97" s="1"/>
       <c r="O97" s="2"/>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>11</v>
       </c>
@@ -10346,7 +11378,7 @@
       </c>
       <c r="L98" s="1"/>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>12</v>
       </c>
@@ -10359,7 +11391,7 @@
       <c r="H99" s="6"/>
       <c r="I99" s="6"/>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>13</v>
       </c>
@@ -10389,7 +11421,7 @@
       </c>
       <c r="L100" s="1"/>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>14</v>
       </c>
@@ -10420,7 +11452,7 @@
       <c r="L101" s="1"/>
       <c r="O101" s="2"/>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>15</v>
       </c>
@@ -10433,7 +11465,7 @@
       <c r="H102" s="6"/>
       <c r="I102" s="6"/>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>16</v>
       </c>
@@ -10462,7 +11494,7 @@
         <v>10131</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>17</v>
       </c>
@@ -10491,7 +11523,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>18</v>
       </c>
@@ -10520,7 +11552,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>19</v>
       </c>
@@ -10549,8 +11581,56 @@
         <v>10178</v>
       </c>
       <c r="L106" s="1"/>
-    </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="AF106">
+        <v>1</v>
+      </c>
+      <c r="AG106">
+        <v>2</v>
+      </c>
+      <c r="AH106">
+        <v>4</v>
+      </c>
+      <c r="AI106">
+        <v>8</v>
+      </c>
+      <c r="AJ106">
+        <v>16</v>
+      </c>
+      <c r="AK106">
+        <v>32</v>
+      </c>
+      <c r="AL106">
+        <v>64</v>
+      </c>
+      <c r="AM106">
+        <v>128</v>
+      </c>
+      <c r="AQ106">
+        <v>1</v>
+      </c>
+      <c r="AR106">
+        <v>2</v>
+      </c>
+      <c r="AS106">
+        <v>4</v>
+      </c>
+      <c r="AT106">
+        <v>8</v>
+      </c>
+      <c r="AU106">
+        <v>16</v>
+      </c>
+      <c r="AV106">
+        <v>32</v>
+      </c>
+      <c r="AW106">
+        <v>64</v>
+      </c>
+      <c r="AX106">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="107" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>20</v>
       </c>
@@ -10578,8 +11658,86 @@
       <c r="I107" s="6">
         <v>320</v>
       </c>
-    </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="W107">
+        <v>1</v>
+      </c>
+      <c r="X107">
+        <v>2</v>
+      </c>
+      <c r="Y107">
+        <v>4</v>
+      </c>
+      <c r="Z107">
+        <v>8</v>
+      </c>
+      <c r="AA107">
+        <v>16</v>
+      </c>
+      <c r="AB107">
+        <v>32</v>
+      </c>
+      <c r="AC107">
+        <v>64</v>
+      </c>
+      <c r="AD107">
+        <v>128</v>
+      </c>
+      <c r="AE107" t="s">
+        <v>72</v>
+      </c>
+      <c r="AF107" s="6">
+        <v>3457942</v>
+      </c>
+      <c r="AG107" s="6">
+        <v>3416827</v>
+      </c>
+      <c r="AH107" s="6">
+        <v>7830031</v>
+      </c>
+      <c r="AI107" s="6">
+        <v>3385509</v>
+      </c>
+      <c r="AJ107" s="6">
+        <v>868520</v>
+      </c>
+      <c r="AK107" s="6">
+        <v>817838</v>
+      </c>
+      <c r="AL107" s="6">
+        <v>830026</v>
+      </c>
+      <c r="AM107" s="6">
+        <v>933362</v>
+      </c>
+      <c r="AP107" t="s">
+        <v>8</v>
+      </c>
+      <c r="AQ107" s="6">
+        <v>3081</v>
+      </c>
+      <c r="AR107" s="6">
+        <v>1253</v>
+      </c>
+      <c r="AS107" s="6">
+        <v>775</v>
+      </c>
+      <c r="AT107" s="6">
+        <v>968</v>
+      </c>
+      <c r="AU107" s="6">
+        <v>902</v>
+      </c>
+      <c r="AV107" s="6">
+        <v>760</v>
+      </c>
+      <c r="AW107" s="6">
+        <v>706</v>
+      </c>
+      <c r="AX107" s="6">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="108" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>22</v>
       </c>
@@ -10608,8 +11766,62 @@
         <v>14135</v>
       </c>
       <c r="L108" s="1"/>
-    </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="AE108" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF108" s="6">
+        <v>1838813</v>
+      </c>
+      <c r="AG108" s="6">
+        <v>1690111</v>
+      </c>
+      <c r="AH108" s="6">
+        <v>1007093</v>
+      </c>
+      <c r="AI108" s="6">
+        <v>730487</v>
+      </c>
+      <c r="AJ108" s="6">
+        <v>267862</v>
+      </c>
+      <c r="AK108" s="6">
+        <v>243491</v>
+      </c>
+      <c r="AL108" s="6">
+        <v>226570</v>
+      </c>
+      <c r="AM108" s="6">
+        <v>233753</v>
+      </c>
+      <c r="AP108" t="s">
+        <v>72</v>
+      </c>
+      <c r="AQ108">
+        <v>3221</v>
+      </c>
+      <c r="AR108">
+        <v>2827</v>
+      </c>
+      <c r="AS108">
+        <v>3832</v>
+      </c>
+      <c r="AT108">
+        <v>5407</v>
+      </c>
+      <c r="AU108">
+        <v>7180</v>
+      </c>
+      <c r="AV108">
+        <v>10164</v>
+      </c>
+      <c r="AW108">
+        <v>13132</v>
+      </c>
+      <c r="AX108">
+        <v>10299</v>
+      </c>
+    </row>
+    <row r="109" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>23</v>
       </c>
@@ -10622,8 +11834,35 @@
       <c r="H109" s="6"/>
       <c r="I109" s="6"/>
       <c r="L109" s="1"/>
-    </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="V109" t="s">
+        <v>89</v>
+      </c>
+      <c r="W109">
+        <v>3503</v>
+      </c>
+      <c r="X109">
+        <v>3364</v>
+      </c>
+      <c r="Y109">
+        <v>5425</v>
+      </c>
+      <c r="Z109">
+        <v>8337</v>
+      </c>
+      <c r="AA109">
+        <v>13407</v>
+      </c>
+      <c r="AB109">
+        <v>23888</v>
+      </c>
+      <c r="AC109">
+        <v>40767</v>
+      </c>
+      <c r="AD109">
+        <v>38376</v>
+      </c>
+    </row>
+    <row r="110" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>24</v>
       </c>
@@ -10637,8 +11876,35 @@
       <c r="I110" s="6"/>
       <c r="L110" s="1"/>
       <c r="O110" s="2"/>
-    </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="V110" t="s">
+        <v>90</v>
+      </c>
+      <c r="W110" s="6">
+        <v>3346</v>
+      </c>
+      <c r="X110" s="6">
+        <v>1404</v>
+      </c>
+      <c r="Y110" s="6">
+        <v>1046</v>
+      </c>
+      <c r="Z110" s="6">
+        <v>1351</v>
+      </c>
+      <c r="AA110" s="6">
+        <v>1113</v>
+      </c>
+      <c r="AB110" s="6">
+        <v>848</v>
+      </c>
+      <c r="AC110" s="6">
+        <v>1082</v>
+      </c>
+      <c r="AD110" s="6">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="111" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>25</v>
       </c>
@@ -10653,7 +11919,7 @@
       <c r="L111" s="1"/>
       <c r="O111" s="2"/>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>26</v>
       </c>

</xml_diff>